<commit_message>
pegando cep e skus da planilha base
</commit_message>
<xml_diff>
--- a/dados_transportadoras_vtex.xlsx
+++ b/dados_transportadoras_vtex.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,75 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>88134360</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2071060</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Retira - SC PALHOCA - Loja Palhoça (30)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1bd</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Grátis</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>88134360</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2071060</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Retira - SC SAO JOSE - Loja Campinas (1)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1bd</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Grátis</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>88134360</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2071060</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Entrega SC</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4bd</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>R$ 29.65</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>